<commit_message>
Stock Card Report - add xlsx templates, update the generated report, fix conditions in query, fix dropdown values
</commit_message>
<xml_diff>
--- a/public/excel_templates/stock-card-report-template.xlsx
+++ b/public/excel_templates/stock-card-report-template.xlsx
@@ -26,12 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
-    <t>Unlimited Network of Opportunities International Corp.</t>
-  </si>
-  <si>
-    <t>TIN: 132-123-012 VAT</t>
-  </si>
-  <si>
     <t>Date Printed:</t>
   </si>
   <si>
@@ -51,6 +45,12 @@
   </si>
   <si>
     <t>Bal</t>
+  </si>
+  <si>
+    <t>UNO International Corp / UNO Premier Philippines International Corp</t>
+  </si>
+  <si>
+    <t>TIN: 006-505-014 VAT / 008-902-716 VAT</t>
   </si>
 </sst>
 </file>
@@ -396,7 +396,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -407,17 +407,17 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -433,25 +433,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>